<commit_message>
Explorar los genes en las enfermedades raras y neurológicas
Se agregó la funcionalidad para explorar la relación entre genes y enfermedades raras y neurológicas. Esto incluye la creación de tablas específicas que mapean los genes a sus correspondientes nombres de enfermedades. Se implementaron heatmaps para visualizar la frecuencia de genes asociados con estas enfermedades, facilitando así el análisis comparativo entre diferentes categorías de enfermedades. Esta mejora optimiza la representación de datos y permite una exploración más detallada de las conexiones genéticas.
</commit_message>
<xml_diff>
--- a/5_Integración con datos de patógenos y enfermedades/Identificación de genes comunes entre probióticos/genes_multiple_categories_final.xlsx
+++ b/5_Integración con datos de patógenos y enfermedades/Identificación de genes comunes entre probióticos/genes_multiple_categories_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PLK2</t>
+          <t>THBS1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Associated with Dysbiosis, Cancer, Neurological Diseases, Rare Diseases</t>
+          <t>Associated with Dysbiosis, Cancer, Neurological Diseases, Rare Diseases, Viral Diseases</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,17 +470,34 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>THBS1</t>
+          <t>PLK2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Associated with Dysbiosis, Cancer, Neurological Diseases, Rare Diseases, Viral Diseases</t>
+          <t>Associated with Dysbiosis, Cancer, Neurological Diseases, Rare Diseases</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Bacillus, Fusobacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CXCL8</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Associated with Dysbiosis, Cancer, Neurological Diseases, Pathogenic Bacteria, Rare Diseases, Viral Diseases</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bacillus, Lactobacillus</t>
         </is>
       </c>
     </row>

</xml_diff>